<commit_message>
improve code PI update,create for admin
</commit_message>
<xml_diff>
--- a/public/Workload.xlsx
+++ b/public/Workload.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -89,9 +88,6 @@
     <t>Giảng viên cơ hữu/Bán cơ hữu</t>
   </si>
   <si>
-    <t>CNTT</t>
-  </si>
-  <si>
     <t>K19T1,2</t>
   </si>
   <si>
@@ -117,6 +113,9 @@
   </si>
   <si>
     <t>MÃ KHOA</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
 </sst>
 </file>
@@ -646,7 +645,7 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -665,7 +664,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="25.5">
       <c r="A1" s="36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
@@ -702,10 +701,10 @@
     </row>
     <row r="3" spans="1:16" ht="26.25" customHeight="1">
       <c r="A3" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="34" t="s">
         <v>22</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>23</v>
       </c>
       <c r="C3" s="32"/>
       <c r="D3" s="32"/>
@@ -804,7 +803,7 @@
         <v>13</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P6" s="31" t="s">
         <v>18</v>
@@ -837,16 +836,16 @@
         <v>1</v>
       </c>
       <c r="B8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="E8" s="14" t="s">
         <v>27</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>28</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>16</v>
@@ -858,7 +857,7 @@
         <v>60</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J8" s="17">
         <v>50</v>
@@ -874,7 +873,7 @@
       </c>
       <c r="N8" s="20"/>
       <c r="O8" s="21" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="P8" s="23">
         <v>1</v>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' of https://github.com/n24xxx/PortalVLU"
This reverts commit 86422995d94a100700649ee63d12ee5de611ec1d, reversing
changes made to 14830a2a7dd2d607479a8eb1b8950743df4c20a5.
</commit_message>
<xml_diff>
--- a/public/Workload.xlsx
+++ b/public/Workload.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -88,6 +89,9 @@
     <t>Giảng viên cơ hữu/Bán cơ hữu</t>
   </si>
   <si>
+    <t>CNTT</t>
+  </si>
+  <si>
     <t>K19T1,2</t>
   </si>
   <si>
@@ -113,9 +117,6 @@
   </si>
   <si>
     <t>MÃ KHOA</t>
-  </si>
-  <si>
-    <t>T</t>
   </si>
 </sst>
 </file>
@@ -645,7 +646,7 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -664,7 +665,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="25.5">
       <c r="A1" s="36" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
@@ -701,10 +702,10 @@
     </row>
     <row r="3" spans="1:16" ht="26.25" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" s="32"/>
       <c r="D3" s="32"/>
@@ -803,7 +804,7 @@
         <v>13</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P6" s="31" t="s">
         <v>18</v>
@@ -836,16 +837,16 @@
         <v>1</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="14" t="s">
-        <v>25</v>
-      </c>
       <c r="E8" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>16</v>
@@ -857,7 +858,7 @@
         <v>60</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J8" s="17">
         <v>50</v>
@@ -873,7 +874,7 @@
       </c>
       <c r="N8" s="20"/>
       <c r="O8" s="21" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="P8" s="23">
         <v>1</v>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' of https://github.com/n24xxx/PortalVLU""
This reverts commit 016227f5e18ba8026eb594e921c4c69472afe65d.
</commit_message>
<xml_diff>
--- a/public/Workload.xlsx
+++ b/public/Workload.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -89,9 +88,6 @@
     <t>Giảng viên cơ hữu/Bán cơ hữu</t>
   </si>
   <si>
-    <t>CNTT</t>
-  </si>
-  <si>
     <t>K19T1,2</t>
   </si>
   <si>
@@ -117,6 +113,9 @@
   </si>
   <si>
     <t>MÃ KHOA</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
 </sst>
 </file>
@@ -646,7 +645,7 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -665,7 +664,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="25.5">
       <c r="A1" s="36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
@@ -702,10 +701,10 @@
     </row>
     <row r="3" spans="1:16" ht="26.25" customHeight="1">
       <c r="A3" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="34" t="s">
         <v>22</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>23</v>
       </c>
       <c r="C3" s="32"/>
       <c r="D3" s="32"/>
@@ -804,7 +803,7 @@
         <v>13</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P6" s="31" t="s">
         <v>18</v>
@@ -837,16 +836,16 @@
         <v>1</v>
       </c>
       <c r="B8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="E8" s="14" t="s">
         <v>27</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>28</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>16</v>
@@ -858,7 +857,7 @@
         <v>60</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J8" s="17">
         <v>50</v>
@@ -874,7 +873,7 @@
       </c>
       <c r="N8" s="20"/>
       <c r="O8" s="21" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="P8" s="23">
         <v>1</v>

</xml_diff>